<commit_message>
Usuniecie ostrzezenia o stopce w szablonie raportu, usuwanie duplikatów z listy relacji
</commit_message>
<xml_diff>
--- a/raport/szablon_raport_z_importu.xlsx
+++ b/raport/szablon_raport_z_importu.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoxy\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\QMapa\raport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geoxy\AppData\Roaming\QGIS\QGIS3\profiles\default\python\plugins\QMapa\raport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="QMapa_import" sheetId="2" r:id="rId1"/>
@@ -877,46 +877,46 @@
     <xf numFmtId="3" fontId="23" fillId="28" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="23" fillId="28" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="28" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="28" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="28" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="18" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1011,7 @@
         <xdr:cNvPr id="2" name="Obraz 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,19 +1343,19 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="3" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" style="12" customWidth="1"/>
-    <col min="5" max="8" width="12.6640625" style="13" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="3.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" style="12" customWidth="1"/>
+    <col min="5" max="8" width="12.7109375" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1364,7 +1364,7 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1372,14 +1372,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H3" s="36"/>
     </row>
-    <row r="4" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>6</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1417,7 +1417,7 @@
       <c r="F8" s="16"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -1428,14 +1428,14 @@
       <c r="G9" s="16"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+    <row r="10" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="67" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="53" t="s">
@@ -1444,14 +1444,14 @@
       <c r="E10" s="54"/>
       <c r="F10" s="55"/>
       <c r="G10" s="56"/>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
+    <row r="11" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="69"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="50" t="s">
         <v>16</v>
       </c>
@@ -1464,12 +1464,12 @@
       <c r="G11" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="60"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="59"/>
+      <c r="H11" s="57"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="51" t="s">
         <v>18</v>
       </c>
@@ -1478,9 +1478,9 @@
       <c r="G12" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="60"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="57"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="2"/>
       <c r="C13" s="29"/>
@@ -1490,7 +1490,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>2</v>
       </c>
@@ -1501,7 +1501,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
     </row>
-    <row r="15" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="E15" s="16"/>
@@ -1509,7 +1509,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="16" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20"/>
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
@@ -1518,19 +1518,19 @@
       <c r="G16" s="41"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="63" t="s">
+    <row r="19" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="67" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="46" t="s">
@@ -1539,14 +1539,14 @@
       <c r="E19" s="47"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
-      <c r="H19" s="60" t="s">
+      <c r="H19" s="57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="59"/>
+    <row r="20" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="50" t="s">
         <v>16</v>
       </c>
@@ -1559,12 +1559,12 @@
       <c r="G20" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="60"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="61"/>
+      <c r="H20" s="57"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="51" t="s">
         <v>18</v>
       </c>
@@ -1573,9 +1573,9 @@
       <c r="G21" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="62"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="58"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
@@ -1585,7 +1585,7 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>2</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="C24" s="19"/>
       <c r="E24" s="16"/>
@@ -1604,7 +1604,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="24"/>
       <c r="C25" s="42"/>
       <c r="D25" s="43"/>
@@ -1613,19 +1613,19 @@
       <c r="G25" s="41"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="27" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="69" t="s">
+    <row r="28" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="70" t="s">
+      <c r="B28" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="67" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="46" t="s">
@@ -1634,14 +1634,14 @@
       <c r="E28" s="47"/>
       <c r="F28" s="48"/>
       <c r="G28" s="49"/>
-      <c r="H28" s="60" t="s">
+      <c r="H28" s="57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="69"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="59"/>
+    <row r="29" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="65"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="67"/>
       <c r="D29" s="50" t="s">
         <v>16</v>
       </c>
@@ -1654,12 +1654,12 @@
       <c r="G29" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="60"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="69"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="61"/>
+      <c r="H29" s="57"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="65"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="68"/>
       <c r="D30" s="51" t="s">
         <v>18</v>
       </c>
@@ -1668,9 +1668,9 @@
       <c r="G30" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H30" s="62"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="58"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="25"/>
       <c r="C31" s="22"/>
@@ -1680,7 +1680,7 @@
       <c r="G31" s="23"/>
       <c r="H31" s="23"/>
     </row>
-    <row r="32" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
         <v>2</v>
       </c>
@@ -1691,7 +1691,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
       <c r="E33" s="16"/>
@@ -1699,7 +1699,7 @@
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="26"/>
       <c r="C34" s="40"/>
       <c r="D34" s="41"/>
@@ -1708,19 +1708,19 @@
       <c r="G34" s="41"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="36" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="65" t="s">
+    <row r="37" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="66" t="s">
+      <c r="B37" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="63" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="27"/>
@@ -1729,17 +1729,17 @@
       <c r="G37" s="27"/>
       <c r="H37" s="27"/>
     </row>
-    <row r="38" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="65"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="68"/>
+    <row r="38" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="61"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="64"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="38"/>
       <c r="B39" s="39"/>
       <c r="C39" s="22"/>
@@ -1749,7 +1749,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
     </row>
-    <row r="40" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="17" t="s">
         <v>2</v>
       </c>
@@ -1762,6 +1762,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="H19:H21"/>
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="B19:B21"/>
@@ -1771,18 +1777,9 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="H19:H21"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>Strona &amp;P z &amp;N</oddFooter>
-  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
poprawka roku na 2024 w raporcie, przygotowanie tekstow do requestow
</commit_message>
<xml_diff>
--- a/raport/szablon_raport_z_importu.xlsx
+++ b/raport/szablon_raport_z_importu.xlsx
@@ -37,9 +37,6 @@
     <t>archiwalne</t>
   </si>
   <si>
-    <t>© 2022 GEOXY sp. z o.o.</t>
-  </si>
-  <si>
     <t>modyfikowane</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve">Obiekty niestandardowe </t>
+  </si>
+  <si>
+    <t>© 2024 GEOXY sp. z o.o.</t>
   </si>
 </sst>
 </file>
@@ -878,9 +878,21 @@
     <xf numFmtId="3" fontId="23" fillId="28" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="28" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="23" fillId="28" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="22" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="23" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -906,18 +918,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="28" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="28" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1012,7 +1012,7 @@
         <xdr:cNvPr id="2" name="Obraz 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15A37402-D866-0FDD-4B11-9268CBD4FA76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,10 +1365,10 @@
     </row>
     <row r="2" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1380,7 +1380,7 @@
     </row>
     <row r="5" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="12"/>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="6" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="12"/>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="7" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="12"/>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="9" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1428,56 +1428,56 @@
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="67" t="s">
-        <v>14</v>
+      <c r="C10" s="59" t="s">
+        <v>13</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="54"/>
       <c r="F10" s="55"/>
       <c r="G10" s="56"/>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="57"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="50" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="50" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" s="50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" s="50" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="60"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="57"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="51" t="s">
         <v>17</v>
-      </c>
-      <c r="H11" s="57"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="51" t="s">
-        <v>18</v>
       </c>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
       <c r="G12" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="57"/>
+        <v>18</v>
+      </c>
+      <c r="H12" s="60"/>
     </row>
     <row r="13" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32"/>
@@ -1519,60 +1519,60 @@
     </row>
     <row r="18" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="67" t="s">
-        <v>14</v>
+      <c r="C19" s="59" t="s">
+        <v>13</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="47"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
-      <c r="H19" s="57" t="s">
+      <c r="H19" s="60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="63"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="50" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="59"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="50" t="s">
-        <v>16</v>
-      </c>
       <c r="E20" s="50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="50" t="s">
         <v>3</v>
       </c>
       <c r="G20" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="60"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="63"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="51" t="s">
         <v>17</v>
-      </c>
-      <c r="H20" s="57"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="51" t="s">
-        <v>18</v>
       </c>
       <c r="E21" s="52"/>
       <c r="F21" s="52"/>
       <c r="G21" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="58"/>
+        <v>18</v>
+      </c>
+      <c r="H21" s="62"/>
     </row>
     <row r="22" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
@@ -1614,60 +1614,60 @@
     </row>
     <row r="27" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="59" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="67" t="s">
-        <v>14</v>
-      </c>
       <c r="D28" s="46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="47"/>
       <c r="F28" s="48"/>
       <c r="G28" s="49"/>
-      <c r="H28" s="57" t="s">
+      <c r="H28" s="60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="69"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="50" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="50" t="s">
-        <v>16</v>
-      </c>
       <c r="E29" s="50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" s="50" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="60"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="69"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="51" t="s">
         <v>17</v>
-      </c>
-      <c r="H29" s="57"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="51" t="s">
-        <v>18</v>
       </c>
       <c r="E30" s="52"/>
       <c r="F30" s="52"/>
       <c r="G30" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="58"/>
+        <v>18</v>
+      </c>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34"/>
@@ -1709,18 +1709,18 @@
     </row>
     <row r="36" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="63" t="s">
-        <v>15</v>
+      <c r="C37" s="67" t="s">
+        <v>14</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
@@ -1729,9 +1729,9 @@
       <c r="H37" s="27"/>
     </row>
     <row r="38" spans="1:8" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="61"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="64"/>
+      <c r="A38" s="65"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="68"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
@@ -1761,12 +1761,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="H19:H21"/>
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="B19:B21"/>
@@ -1776,6 +1770,12 @@
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="H19:H21"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>